<commit_message>
feat: add batch job applications from 2/26-2/27 intake
45 new application folders with metadata, job descriptions, and match
scores. Updated tracker, index, and memory.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K302"/>
+  <dimension ref="A1:K348"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -829,8 +829,6 @@
           <t>Evaluating</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Saved. Cover letter created on 2026-02-17.</t>
@@ -863,8 +861,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-02-12.</t>
@@ -897,8 +893,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-02-04.</t>
@@ -931,8 +925,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-02-04.</t>
@@ -965,8 +957,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -999,8 +989,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-02-04.</t>
@@ -1033,8 +1021,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-05.</t>
@@ -1067,8 +1053,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-02-04.</t>
@@ -1101,8 +1085,6 @@
           <t>Interviewing</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Interviewing. Cover letter created on 2026-01-28.</t>
@@ -1135,8 +1117,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-23.</t>
@@ -1169,8 +1149,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-23.</t>
@@ -1203,8 +1181,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-23.</t>
@@ -1237,8 +1213,6 @@
           <t>Interviewing</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Interviewing. Cover letter created on 2026-01-23.</t>
@@ -1271,8 +1245,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-23.</t>
@@ -1305,8 +1277,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-23.</t>
@@ -1339,8 +1309,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-23.</t>
@@ -1373,8 +1341,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-23.</t>
@@ -1407,8 +1373,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-23.</t>
@@ -1441,8 +1405,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-23.</t>
@@ -1475,8 +1437,6 @@
           <t>Interviewing</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Interviewing. Cover letter created on 2026-01-22.</t>
@@ -1509,8 +1469,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -1543,8 +1501,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -1577,8 +1533,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -1611,8 +1565,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -1645,8 +1597,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -1679,8 +1629,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -1713,8 +1661,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -1747,8 +1693,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -1781,8 +1725,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
       <c r="K37" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-21.</t>
@@ -1815,8 +1757,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
       <c r="K38" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-20.</t>
@@ -1849,8 +1789,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
       <c r="K39" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-20.</t>
@@ -1883,8 +1821,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
       <c r="K40" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-20.</t>
@@ -1917,8 +1853,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
       <c r="K41" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-15.</t>
@@ -1951,8 +1885,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
       <c r="K42" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-15.</t>
@@ -1985,8 +1917,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
       <c r="K43" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-15.</t>
@@ -2019,8 +1949,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
       <c r="K44" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-15.</t>
@@ -2053,8 +1981,6 @@
           <t>Interviewing</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
       <c r="K45" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Interviewing. Cover letter created on 2026-01-13.</t>
@@ -2087,8 +2013,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
       <c r="K46" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-13.</t>
@@ -2121,8 +2045,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
       <c r="K47" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-13.</t>
@@ -2155,8 +2077,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
       <c r="K48" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-13.</t>
@@ -2189,8 +2109,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
       <c r="K49" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-13.</t>
@@ -2223,8 +2141,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
       <c r="K50" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-13.</t>
@@ -2257,8 +2173,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
       <c r="K51" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-13.</t>
@@ -2291,8 +2205,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
       <c r="K52" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-07.</t>
@@ -2325,8 +2237,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
       <c r="K53" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-07.</t>
@@ -2359,8 +2269,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
       <c r="K54" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-07.</t>
@@ -2393,8 +2301,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
       <c r="K55" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-07.</t>
@@ -2427,8 +2333,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
       <c r="K56" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-06.</t>
@@ -2461,8 +2365,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
       <c r="K57" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-17.</t>
@@ -2495,8 +2397,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
       <c r="K58" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-06.</t>
@@ -2529,8 +2429,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
       <c r="K59" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-06.</t>
@@ -2563,8 +2461,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr"/>
-      <c r="H60" t="inlineStr"/>
       <c r="K60" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-06.</t>
@@ -2597,8 +2493,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
       <c r="K61" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-06.</t>
@@ -2631,8 +2525,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="H62" t="inlineStr"/>
       <c r="K62" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-06.</t>
@@ -2665,8 +2557,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="H63" t="inlineStr"/>
       <c r="K63" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2026-01-06.</t>
@@ -2699,8 +2589,6 @@
           <t>Interviewing</t>
         </is>
       </c>
-      <c r="F64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
       <c r="K64" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Interviewing. Cover letter created on 2025-12-31.</t>
@@ -2733,8 +2621,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
       <c r="K65" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-29.</t>
@@ -2767,8 +2653,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="H66" t="inlineStr"/>
       <c r="K66" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-29.</t>
@@ -2801,8 +2685,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
       <c r="K67" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-24.</t>
@@ -2835,8 +2717,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="H68" t="inlineStr"/>
       <c r="K68" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-29.</t>
@@ -2869,8 +2749,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="H69" t="inlineStr"/>
       <c r="K69" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-29.</t>
@@ -2903,8 +2781,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
       <c r="K70" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-29.</t>
@@ -2937,8 +2813,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="H71" t="inlineStr"/>
       <c r="K71" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-29.</t>
@@ -2971,8 +2845,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
       <c r="K72" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-24.</t>
@@ -3005,8 +2877,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="H73" t="inlineStr"/>
       <c r="K73" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-24.</t>
@@ -3039,8 +2909,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="H74" t="inlineStr"/>
       <c r="K74" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-24.</t>
@@ -3073,8 +2941,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="H75" t="inlineStr"/>
       <c r="K75" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-24.</t>
@@ -3107,8 +2973,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="H76" t="inlineStr"/>
       <c r="K76" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-24.</t>
@@ -3141,8 +3005,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="H77" t="inlineStr"/>
       <c r="K77" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-24.</t>
@@ -3175,8 +3037,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr"/>
-      <c r="H78" t="inlineStr"/>
       <c r="K78" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-21.</t>
@@ -3209,8 +3069,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr"/>
-      <c r="H79" t="inlineStr"/>
       <c r="K79" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-19.</t>
@@ -3243,8 +3101,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F80" t="inlineStr"/>
-      <c r="H80" t="inlineStr"/>
       <c r="K80" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-19.</t>
@@ -3277,8 +3133,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="H81" t="inlineStr"/>
       <c r="K81" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-17.</t>
@@ -3311,8 +3165,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr"/>
-      <c r="H82" t="inlineStr"/>
       <c r="K82" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-17.</t>
@@ -3345,8 +3197,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
       <c r="K83" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-17.</t>
@@ -3379,8 +3229,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr"/>
-      <c r="H84" t="inlineStr"/>
       <c r="K84" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-17.</t>
@@ -3413,8 +3261,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr"/>
-      <c r="H85" t="inlineStr"/>
       <c r="K85" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-17.</t>
@@ -3447,8 +3293,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr"/>
-      <c r="H86" t="inlineStr"/>
       <c r="K86" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-17.</t>
@@ -3481,8 +3325,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F87" t="inlineStr"/>
-      <c r="H87" t="inlineStr"/>
       <c r="K87" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-15.</t>
@@ -3515,8 +3357,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F88" t="inlineStr"/>
-      <c r="H88" t="inlineStr"/>
       <c r="K88" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-15.</t>
@@ -3549,8 +3389,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F89" t="inlineStr"/>
-      <c r="H89" t="inlineStr"/>
       <c r="K89" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-15.</t>
@@ -3583,8 +3421,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr"/>
-      <c r="H90" t="inlineStr"/>
       <c r="K90" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-15.</t>
@@ -3617,8 +3453,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="H91" t="inlineStr"/>
       <c r="K91" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-08.</t>
@@ -3651,8 +3485,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F92" t="inlineStr"/>
-      <c r="H92" t="inlineStr"/>
       <c r="K92" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-08.</t>
@@ -3685,8 +3517,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="H93" t="inlineStr"/>
       <c r="K93" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-12-05.</t>
@@ -3719,8 +3549,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr"/>
-      <c r="H94" t="inlineStr"/>
       <c r="K94" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-11-21.</t>
@@ -3753,8 +3581,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr"/>
-      <c r="H95" t="inlineStr"/>
       <c r="K95" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-11-21.</t>
@@ -3787,8 +3613,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F96" t="inlineStr"/>
-      <c r="H96" t="inlineStr"/>
       <c r="K96" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-11-21.</t>
@@ -3821,8 +3645,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
       <c r="K97" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-11-21.</t>
@@ -3855,8 +3677,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr"/>
-      <c r="H98" t="inlineStr"/>
       <c r="K98" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-11-21.</t>
@@ -3889,8 +3709,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr"/>
-      <c r="H99" t="inlineStr"/>
       <c r="K99" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied. Cover letter created on 2025-11-21.</t>
@@ -3923,8 +3741,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F100" t="inlineStr"/>
-      <c r="H100" t="inlineStr"/>
       <c r="K100" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -3957,8 +3773,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr"/>
-      <c r="H101" t="inlineStr"/>
       <c r="K101" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -3991,8 +3805,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr"/>
-      <c r="H102" t="inlineStr"/>
       <c r="K102" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4025,8 +3837,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr"/>
-      <c r="H103" t="inlineStr"/>
       <c r="K103" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4059,8 +3869,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr"/>
-      <c r="H104" t="inlineStr"/>
       <c r="K104" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4093,8 +3901,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr"/>
-      <c r="H105" t="inlineStr"/>
       <c r="K105" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4127,8 +3933,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr"/>
-      <c r="H106" t="inlineStr"/>
       <c r="K106" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4161,8 +3965,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr"/>
-      <c r="H107" t="inlineStr"/>
       <c r="K107" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4195,8 +3997,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F108" t="inlineStr"/>
-      <c r="H108" t="inlineStr"/>
       <c r="K108" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4229,8 +4029,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr"/>
-      <c r="H109" t="inlineStr"/>
       <c r="K109" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4263,8 +4061,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F110" t="inlineStr"/>
-      <c r="H110" t="inlineStr"/>
       <c r="K110" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4297,8 +4093,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr"/>
-      <c r="H111" t="inlineStr"/>
       <c r="K111" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4331,8 +4125,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr"/>
-      <c r="H112" t="inlineStr"/>
       <c r="K112" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4365,8 +4157,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F113" t="inlineStr"/>
-      <c r="H113" t="inlineStr"/>
       <c r="K113" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4399,8 +4189,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F114" t="inlineStr"/>
-      <c r="H114" t="inlineStr"/>
       <c r="K114" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4433,8 +4221,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F115" t="inlineStr"/>
-      <c r="H115" t="inlineStr"/>
       <c r="K115" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4467,8 +4253,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F116" t="inlineStr"/>
-      <c r="H116" t="inlineStr"/>
       <c r="K116" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4501,8 +4285,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F117" t="inlineStr"/>
-      <c r="H117" t="inlineStr"/>
       <c r="K117" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4535,8 +4317,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F118" t="inlineStr"/>
-      <c r="H118" t="inlineStr"/>
       <c r="K118" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4569,8 +4349,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F119" t="inlineStr"/>
-      <c r="H119" t="inlineStr"/>
       <c r="K119" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4603,8 +4381,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F120" t="inlineStr"/>
-      <c r="H120" t="inlineStr"/>
       <c r="K120" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4637,8 +4413,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr"/>
-      <c r="H121" t="inlineStr"/>
       <c r="K121" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4671,8 +4445,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F122" t="inlineStr"/>
-      <c r="H122" t="inlineStr"/>
       <c r="K122" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4705,8 +4477,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F123" t="inlineStr"/>
-      <c r="H123" t="inlineStr"/>
       <c r="K123" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4739,8 +4509,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F124" t="inlineStr"/>
-      <c r="H124" t="inlineStr"/>
       <c r="K124" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4773,8 +4541,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F125" t="inlineStr"/>
-      <c r="H125" t="inlineStr"/>
       <c r="K125" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4807,8 +4573,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F126" t="inlineStr"/>
-      <c r="H126" t="inlineStr"/>
       <c r="K126" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4841,8 +4605,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F127" t="inlineStr"/>
-      <c r="H127" t="inlineStr"/>
       <c r="K127" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4875,8 +4637,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F128" t="inlineStr"/>
-      <c r="H128" t="inlineStr"/>
       <c r="K128" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4909,8 +4669,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F129" t="inlineStr"/>
-      <c r="H129" t="inlineStr"/>
       <c r="K129" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4943,8 +4701,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F130" t="inlineStr"/>
-      <c r="H130" t="inlineStr"/>
       <c r="K130" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -4977,8 +4733,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F131" t="inlineStr"/>
-      <c r="H131" t="inlineStr"/>
       <c r="K131" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5011,8 +4765,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F132" t="inlineStr"/>
-      <c r="H132" t="inlineStr"/>
       <c r="K132" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5045,8 +4797,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F133" t="inlineStr"/>
-      <c r="H133" t="inlineStr"/>
       <c r="K133" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5079,8 +4829,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F134" t="inlineStr"/>
-      <c r="H134" t="inlineStr"/>
       <c r="K134" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5113,8 +4861,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F135" t="inlineStr"/>
-      <c r="H135" t="inlineStr"/>
       <c r="K135" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5147,8 +4893,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F136" t="inlineStr"/>
-      <c r="H136" t="inlineStr"/>
       <c r="K136" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5181,8 +4925,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F137" t="inlineStr"/>
-      <c r="H137" t="inlineStr"/>
       <c r="K137" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5215,8 +4957,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F138" t="inlineStr"/>
-      <c r="H138" t="inlineStr"/>
       <c r="K138" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5249,8 +4989,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F139" t="inlineStr"/>
-      <c r="H139" t="inlineStr"/>
       <c r="K139" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5283,8 +5021,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F140" t="inlineStr"/>
-      <c r="H140" t="inlineStr"/>
       <c r="K140" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5317,8 +5053,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F141" t="inlineStr"/>
-      <c r="H141" t="inlineStr"/>
       <c r="K141" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5351,8 +5085,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F142" t="inlineStr"/>
-      <c r="H142" t="inlineStr"/>
       <c r="K142" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5385,8 +5117,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F143" t="inlineStr"/>
-      <c r="H143" t="inlineStr"/>
       <c r="K143" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5419,8 +5149,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F144" t="inlineStr"/>
-      <c r="H144" t="inlineStr"/>
       <c r="K144" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5453,8 +5181,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F145" t="inlineStr"/>
-      <c r="H145" t="inlineStr"/>
       <c r="K145" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5487,8 +5213,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F146" t="inlineStr"/>
-      <c r="H146" t="inlineStr"/>
       <c r="K146" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5521,8 +5245,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F147" t="inlineStr"/>
-      <c r="H147" t="inlineStr"/>
       <c r="K147" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5555,8 +5277,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F148" t="inlineStr"/>
-      <c r="H148" t="inlineStr"/>
       <c r="K148" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5589,8 +5309,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F149" t="inlineStr"/>
-      <c r="H149" t="inlineStr"/>
       <c r="K149" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5623,8 +5341,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F150" t="inlineStr"/>
-      <c r="H150" t="inlineStr"/>
       <c r="K150" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5657,8 +5373,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F151" t="inlineStr"/>
-      <c r="H151" t="inlineStr"/>
       <c r="K151" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5691,8 +5405,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F152" t="inlineStr"/>
-      <c r="H152" t="inlineStr"/>
       <c r="K152" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5725,8 +5437,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F153" t="inlineStr"/>
-      <c r="H153" t="inlineStr"/>
       <c r="K153" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5759,8 +5469,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F154" t="inlineStr"/>
-      <c r="H154" t="inlineStr"/>
       <c r="K154" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5793,8 +5501,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F155" t="inlineStr"/>
-      <c r="H155" t="inlineStr"/>
       <c r="K155" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5827,8 +5533,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F156" t="inlineStr"/>
-      <c r="H156" t="inlineStr"/>
       <c r="K156" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5861,8 +5565,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F157" t="inlineStr"/>
-      <c r="H157" t="inlineStr"/>
       <c r="K157" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5895,8 +5597,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F158" t="inlineStr"/>
-      <c r="H158" t="inlineStr"/>
       <c r="K158" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5929,8 +5629,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F159" t="inlineStr"/>
-      <c r="H159" t="inlineStr"/>
       <c r="K159" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5963,8 +5661,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F160" t="inlineStr"/>
-      <c r="H160" t="inlineStr"/>
       <c r="K160" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -5997,8 +5693,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F161" t="inlineStr"/>
-      <c r="H161" t="inlineStr"/>
       <c r="K161" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6031,8 +5725,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F162" t="inlineStr"/>
-      <c r="H162" t="inlineStr"/>
       <c r="K162" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6065,8 +5757,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F163" t="inlineStr"/>
-      <c r="H163" t="inlineStr"/>
       <c r="K163" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6099,8 +5789,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F164" t="inlineStr"/>
-      <c r="H164" t="inlineStr"/>
       <c r="K164" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6133,8 +5821,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F165" t="inlineStr"/>
-      <c r="H165" t="inlineStr"/>
       <c r="K165" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6167,8 +5853,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F166" t="inlineStr"/>
-      <c r="H166" t="inlineStr"/>
       <c r="K166" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6201,8 +5885,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F167" t="inlineStr"/>
-      <c r="H167" t="inlineStr"/>
       <c r="K167" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6235,8 +5917,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F168" t="inlineStr"/>
-      <c r="H168" t="inlineStr"/>
       <c r="K168" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6269,8 +5949,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F169" t="inlineStr"/>
-      <c r="H169" t="inlineStr"/>
       <c r="K169" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6303,8 +5981,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F170" t="inlineStr"/>
-      <c r="H170" t="inlineStr"/>
       <c r="K170" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6337,8 +6013,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F171" t="inlineStr"/>
-      <c r="H171" t="inlineStr"/>
       <c r="K171" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6371,8 +6045,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F172" t="inlineStr"/>
-      <c r="H172" t="inlineStr"/>
       <c r="K172" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6405,8 +6077,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F173" t="inlineStr"/>
-      <c r="H173" t="inlineStr"/>
       <c r="K173" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6439,8 +6109,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F174" t="inlineStr"/>
-      <c r="H174" t="inlineStr"/>
       <c r="K174" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6473,8 +6141,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F175" t="inlineStr"/>
-      <c r="H175" t="inlineStr"/>
       <c r="K175" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6507,8 +6173,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F176" t="inlineStr"/>
-      <c r="H176" t="inlineStr"/>
       <c r="K176" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6541,8 +6205,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F177" t="inlineStr"/>
-      <c r="H177" t="inlineStr"/>
       <c r="K177" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6575,8 +6237,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F178" t="inlineStr"/>
-      <c r="H178" t="inlineStr"/>
       <c r="K178" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6609,8 +6269,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F179" t="inlineStr"/>
-      <c r="H179" t="inlineStr"/>
       <c r="K179" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6643,8 +6301,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F180" t="inlineStr"/>
-      <c r="H180" t="inlineStr"/>
       <c r="K180" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6677,8 +6333,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F181" t="inlineStr"/>
-      <c r="H181" t="inlineStr"/>
       <c r="K181" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6711,8 +6365,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr"/>
-      <c r="H182" t="inlineStr"/>
       <c r="K182" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6745,8 +6397,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F183" t="inlineStr"/>
-      <c r="H183" t="inlineStr"/>
       <c r="K183" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6779,8 +6429,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F184" t="inlineStr"/>
-      <c r="H184" t="inlineStr"/>
       <c r="K184" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6813,8 +6461,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F185" t="inlineStr"/>
-      <c r="H185" t="inlineStr"/>
       <c r="K185" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6847,8 +6493,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F186" t="inlineStr"/>
-      <c r="H186" t="inlineStr"/>
       <c r="K186" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6881,8 +6525,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F187" t="inlineStr"/>
-      <c r="H187" t="inlineStr"/>
       <c r="K187" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6915,8 +6557,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F188" t="inlineStr"/>
-      <c r="H188" t="inlineStr"/>
       <c r="K188" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6949,8 +6589,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F189" t="inlineStr"/>
-      <c r="H189" t="inlineStr"/>
       <c r="K189" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -6983,8 +6621,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F190" t="inlineStr"/>
-      <c r="H190" t="inlineStr"/>
       <c r="K190" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7017,8 +6653,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F191" t="inlineStr"/>
-      <c r="H191" t="inlineStr"/>
       <c r="K191" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7051,8 +6685,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F192" t="inlineStr"/>
-      <c r="H192" t="inlineStr"/>
       <c r="K192" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7080,8 +6712,6 @@
           <t>Evaluating</t>
         </is>
       </c>
-      <c r="F193" t="inlineStr"/>
-      <c r="H193" t="inlineStr"/>
       <c r="K193" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Saved.</t>
@@ -7114,8 +6744,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F194" t="inlineStr"/>
-      <c r="H194" t="inlineStr"/>
       <c r="K194" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7148,8 +6776,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F195" t="inlineStr"/>
-      <c r="H195" t="inlineStr"/>
       <c r="K195" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7182,8 +6808,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F196" t="inlineStr"/>
-      <c r="H196" t="inlineStr"/>
       <c r="K196" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7216,8 +6840,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F197" t="inlineStr"/>
-      <c r="H197" t="inlineStr"/>
       <c r="K197" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7250,8 +6872,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F198" t="inlineStr"/>
-      <c r="H198" t="inlineStr"/>
       <c r="K198" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7284,8 +6904,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F199" t="inlineStr"/>
-      <c r="H199" t="inlineStr"/>
       <c r="K199" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7313,8 +6931,6 @@
           <t>Evaluating</t>
         </is>
       </c>
-      <c r="F200" t="inlineStr"/>
-      <c r="H200" t="inlineStr"/>
       <c r="K200" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Saved.</t>
@@ -7347,8 +6963,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F201" t="inlineStr"/>
-      <c r="H201" t="inlineStr"/>
       <c r="K201" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7381,8 +6995,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F202" t="inlineStr"/>
-      <c r="H202" t="inlineStr"/>
       <c r="K202" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7410,8 +7022,6 @@
           <t>Evaluating</t>
         </is>
       </c>
-      <c r="F203" t="inlineStr"/>
-      <c r="H203" t="inlineStr"/>
       <c r="K203" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Saved.</t>
@@ -7444,8 +7054,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F204" t="inlineStr"/>
-      <c r="H204" t="inlineStr"/>
       <c r="K204" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7478,8 +7086,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F205" t="inlineStr"/>
-      <c r="H205" t="inlineStr"/>
       <c r="K205" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7512,8 +7118,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F206" t="inlineStr"/>
-      <c r="H206" t="inlineStr"/>
       <c r="K206" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7546,8 +7150,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F207" t="inlineStr"/>
-      <c r="H207" t="inlineStr"/>
       <c r="K207" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7580,8 +7182,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F208" t="inlineStr"/>
-      <c r="H208" t="inlineStr"/>
       <c r="K208" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7614,8 +7214,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F209" t="inlineStr"/>
-      <c r="H209" t="inlineStr"/>
       <c r="K209" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7648,8 +7246,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F210" t="inlineStr"/>
-      <c r="H210" t="inlineStr"/>
       <c r="K210" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7682,8 +7278,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F211" t="inlineStr"/>
-      <c r="H211" t="inlineStr"/>
       <c r="K211" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7716,8 +7310,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F212" t="inlineStr"/>
-      <c r="H212" t="inlineStr"/>
       <c r="K212" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7750,8 +7342,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F213" t="inlineStr"/>
-      <c r="H213" t="inlineStr"/>
       <c r="K213" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7784,8 +7374,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F214" t="inlineStr"/>
-      <c r="H214" t="inlineStr"/>
       <c r="K214" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7818,8 +7406,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F215" t="inlineStr"/>
-      <c r="H215" t="inlineStr"/>
       <c r="K215" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7852,8 +7438,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F216" t="inlineStr"/>
-      <c r="H216" t="inlineStr"/>
       <c r="K216" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7886,8 +7470,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F217" t="inlineStr"/>
-      <c r="H217" t="inlineStr"/>
       <c r="K217" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7920,8 +7502,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F218" t="inlineStr"/>
-      <c r="H218" t="inlineStr"/>
       <c r="K218" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7954,8 +7534,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F219" t="inlineStr"/>
-      <c r="H219" t="inlineStr"/>
       <c r="K219" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -7988,8 +7566,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F220" t="inlineStr"/>
-      <c r="H220" t="inlineStr"/>
       <c r="K220" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8022,8 +7598,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F221" t="inlineStr"/>
-      <c r="H221" t="inlineStr"/>
       <c r="K221" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8056,8 +7630,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F222" t="inlineStr"/>
-      <c r="H222" t="inlineStr"/>
       <c r="K222" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8090,8 +7662,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F223" t="inlineStr"/>
-      <c r="H223" t="inlineStr"/>
       <c r="K223" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8124,8 +7694,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F224" t="inlineStr"/>
-      <c r="H224" t="inlineStr"/>
       <c r="K224" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8158,8 +7726,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F225" t="inlineStr"/>
-      <c r="H225" t="inlineStr"/>
       <c r="K225" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8192,8 +7758,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F226" t="inlineStr"/>
-      <c r="H226" t="inlineStr"/>
       <c r="K226" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8226,8 +7790,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F227" t="inlineStr"/>
-      <c r="H227" t="inlineStr"/>
       <c r="K227" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8260,8 +7822,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F228" t="inlineStr"/>
-      <c r="H228" t="inlineStr"/>
       <c r="K228" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8294,8 +7854,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F229" t="inlineStr"/>
-      <c r="H229" t="inlineStr"/>
       <c r="K229" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8328,8 +7886,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F230" t="inlineStr"/>
-      <c r="H230" t="inlineStr"/>
       <c r="K230" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8362,8 +7918,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F231" t="inlineStr"/>
-      <c r="H231" t="inlineStr"/>
       <c r="K231" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8396,8 +7950,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F232" t="inlineStr"/>
-      <c r="H232" t="inlineStr"/>
       <c r="K232" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8430,8 +7982,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F233" t="inlineStr"/>
-      <c r="H233" t="inlineStr"/>
       <c r="K233" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8464,8 +8014,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F234" t="inlineStr"/>
-      <c r="H234" t="inlineStr"/>
       <c r="K234" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8498,8 +8046,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F235" t="inlineStr"/>
-      <c r="H235" t="inlineStr"/>
       <c r="K235" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8532,8 +8078,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F236" t="inlineStr"/>
-      <c r="H236" t="inlineStr"/>
       <c r="K236" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8566,8 +8110,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F237" t="inlineStr"/>
-      <c r="H237" t="inlineStr"/>
       <c r="K237" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8600,8 +8142,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F238" t="inlineStr"/>
-      <c r="H238" t="inlineStr"/>
       <c r="K238" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8634,8 +8174,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F239" t="inlineStr"/>
-      <c r="H239" t="inlineStr"/>
       <c r="K239" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8668,8 +8206,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F240" t="inlineStr"/>
-      <c r="H240" t="inlineStr"/>
       <c r="K240" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8702,8 +8238,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F241" t="inlineStr"/>
-      <c r="H241" t="inlineStr"/>
       <c r="K241" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8736,8 +8270,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F242" t="inlineStr"/>
-      <c r="H242" t="inlineStr"/>
       <c r="K242" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8770,8 +8302,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F243" t="inlineStr"/>
-      <c r="H243" t="inlineStr"/>
       <c r="K243" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8804,8 +8334,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F244" t="inlineStr"/>
-      <c r="H244" t="inlineStr"/>
       <c r="K244" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8838,8 +8366,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F245" t="inlineStr"/>
-      <c r="H245" t="inlineStr"/>
       <c r="K245" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8872,8 +8398,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F246" t="inlineStr"/>
-      <c r="H246" t="inlineStr"/>
       <c r="K246" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8906,8 +8430,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F247" t="inlineStr"/>
-      <c r="H247" t="inlineStr"/>
       <c r="K247" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8940,8 +8462,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F248" t="inlineStr"/>
-      <c r="H248" t="inlineStr"/>
       <c r="K248" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -8974,8 +8494,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F249" t="inlineStr"/>
-      <c r="H249" t="inlineStr"/>
       <c r="K249" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9008,8 +8526,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F250" t="inlineStr"/>
-      <c r="H250" t="inlineStr"/>
       <c r="K250" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9042,8 +8558,6 @@
           <t>Interviewing</t>
         </is>
       </c>
-      <c r="F251" t="inlineStr"/>
-      <c r="H251" t="inlineStr"/>
       <c r="K251" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Interviewing.</t>
@@ -9076,8 +8590,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F252" t="inlineStr"/>
-      <c r="H252" t="inlineStr"/>
       <c r="K252" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9110,8 +8622,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F253" t="inlineStr"/>
-      <c r="H253" t="inlineStr"/>
       <c r="K253" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9144,8 +8654,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F254" t="inlineStr"/>
-      <c r="H254" t="inlineStr"/>
       <c r="K254" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9178,8 +8686,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F255" t="inlineStr"/>
-      <c r="H255" t="inlineStr"/>
       <c r="K255" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9212,8 +8718,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F256" t="inlineStr"/>
-      <c r="H256" t="inlineStr"/>
       <c r="K256" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9246,8 +8750,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F257" t="inlineStr"/>
-      <c r="H257" t="inlineStr"/>
       <c r="K257" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9280,8 +8782,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F258" t="inlineStr"/>
-      <c r="H258" t="inlineStr"/>
       <c r="K258" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9314,8 +8814,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F259" t="inlineStr"/>
-      <c r="H259" t="inlineStr"/>
       <c r="K259" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9348,8 +8846,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F260" t="inlineStr"/>
-      <c r="H260" t="inlineStr"/>
       <c r="K260" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9382,8 +8878,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F261" t="inlineStr"/>
-      <c r="H261" t="inlineStr"/>
       <c r="K261" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9416,8 +8910,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F262" t="inlineStr"/>
-      <c r="H262" t="inlineStr"/>
       <c r="K262" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9450,8 +8942,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F263" t="inlineStr"/>
-      <c r="H263" t="inlineStr"/>
       <c r="K263" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9484,8 +8974,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F264" t="inlineStr"/>
-      <c r="H264" t="inlineStr"/>
       <c r="K264" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9518,8 +9006,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F265" t="inlineStr"/>
-      <c r="H265" t="inlineStr"/>
       <c r="K265" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9552,8 +9038,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F266" t="inlineStr"/>
-      <c r="H266" t="inlineStr"/>
       <c r="K266" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9586,8 +9070,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F267" t="inlineStr"/>
-      <c r="H267" t="inlineStr"/>
       <c r="K267" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9620,8 +9102,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F268" t="inlineStr"/>
-      <c r="H268" t="inlineStr"/>
       <c r="K268" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9654,8 +9134,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F269" t="inlineStr"/>
-      <c r="H269" t="inlineStr"/>
       <c r="K269" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9688,8 +9166,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F270" t="inlineStr"/>
-      <c r="H270" t="inlineStr"/>
       <c r="K270" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9722,8 +9198,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F271" t="inlineStr"/>
-      <c r="H271" t="inlineStr"/>
       <c r="K271" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9756,8 +9230,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F272" t="inlineStr"/>
-      <c r="H272" t="inlineStr"/>
       <c r="K272" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9790,8 +9262,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F273" t="inlineStr"/>
-      <c r="H273" t="inlineStr"/>
       <c r="K273" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9824,8 +9294,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F274" t="inlineStr"/>
-      <c r="H274" t="inlineStr"/>
       <c r="K274" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9858,8 +9326,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F275" t="inlineStr"/>
-      <c r="H275" t="inlineStr"/>
       <c r="K275" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9892,8 +9358,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F276" t="inlineStr"/>
-      <c r="H276" t="inlineStr"/>
       <c r="K276" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9926,8 +9390,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F277" t="inlineStr"/>
-      <c r="H277" t="inlineStr"/>
       <c r="K277" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9960,8 +9422,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F278" t="inlineStr"/>
-      <c r="H278" t="inlineStr"/>
       <c r="K278" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -9994,8 +9454,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F279" t="inlineStr"/>
-      <c r="H279" t="inlineStr"/>
       <c r="K279" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10028,8 +9486,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F280" t="inlineStr"/>
-      <c r="H280" t="inlineStr"/>
       <c r="K280" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10062,8 +9518,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F281" t="inlineStr"/>
-      <c r="H281" t="inlineStr"/>
       <c r="K281" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10096,8 +9550,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F282" t="inlineStr"/>
-      <c r="H282" t="inlineStr"/>
       <c r="K282" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10130,8 +9582,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F283" t="inlineStr"/>
-      <c r="H283" t="inlineStr"/>
       <c r="K283" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10164,8 +9614,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F284" t="inlineStr"/>
-      <c r="H284" t="inlineStr"/>
       <c r="K284" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10198,8 +9646,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F285" t="inlineStr"/>
-      <c r="H285" t="inlineStr"/>
       <c r="K285" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10232,8 +9678,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F286" t="inlineStr"/>
-      <c r="H286" t="inlineStr"/>
       <c r="K286" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10266,8 +9710,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F287" t="inlineStr"/>
-      <c r="H287" t="inlineStr"/>
       <c r="K287" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10300,8 +9742,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F288" t="inlineStr"/>
-      <c r="H288" t="inlineStr"/>
       <c r="K288" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10334,8 +9774,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F289" t="inlineStr"/>
-      <c r="H289" t="inlineStr"/>
       <c r="K289" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10368,8 +9806,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F290" t="inlineStr"/>
-      <c r="H290" t="inlineStr"/>
       <c r="K290" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10402,8 +9838,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F291" t="inlineStr"/>
-      <c r="H291" t="inlineStr"/>
       <c r="K291" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10436,8 +9870,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F292" t="inlineStr"/>
-      <c r="H292" t="inlineStr"/>
       <c r="K292" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10470,8 +9902,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F293" t="inlineStr"/>
-      <c r="H293" t="inlineStr"/>
       <c r="K293" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10504,8 +9934,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F294" t="inlineStr"/>
-      <c r="H294" t="inlineStr"/>
       <c r="K294" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10538,8 +9966,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F295" t="inlineStr"/>
-      <c r="H295" t="inlineStr"/>
       <c r="K295" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10572,8 +9998,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F296" t="inlineStr"/>
-      <c r="H296" t="inlineStr"/>
       <c r="K296" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10606,8 +10030,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F297" t="inlineStr"/>
-      <c r="H297" t="inlineStr"/>
       <c r="K297" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10640,8 +10062,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F298" t="inlineStr"/>
-      <c r="H298" t="inlineStr"/>
       <c r="K298" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10674,8 +10094,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F299" t="inlineStr"/>
-      <c r="H299" t="inlineStr"/>
       <c r="K299" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10708,8 +10126,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F300" t="inlineStr"/>
-      <c r="H300" t="inlineStr"/>
       <c r="K300" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10742,8 +10158,6 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F301" t="inlineStr"/>
-      <c r="H301" t="inlineStr"/>
       <c r="K301" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
@@ -10776,11 +10190,1498 @@
           <t>Applied</t>
         </is>
       </c>
-      <c r="F302" t="inlineStr"/>
-      <c r="H302" t="inlineStr"/>
       <c r="K302" t="inlineStr">
         <is>
           <t>Imported from Swooped.ai on 2026-02-25. Swooped status: Applied.</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Bloomerang</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Vice President, Engineering</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K303" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Impiricus</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>VP, Engineering</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K304" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Protege</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>VP, Engineering</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K305" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Soni</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Vice President of Engineering</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K306" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Storm3</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Vice President of Engineering</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K307" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Experian</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Vice President, Software Engineering</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K308" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Dynamic Campus</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Chief Information Officer</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>Stretch</t>
+        </is>
+      </c>
+      <c r="K309" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>AlphaPoint</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>VP of Engineering</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K310" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>BeOne Medicines</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Vice President, AI &amp; Innovation</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K311" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Cooper University Health Care</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>CHIEF AI OFFICER</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K312" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Core Clinical Partners</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Senior Director of IT</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K313" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Expedite Talent Solutions</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Lead Director, Software Development Engineering</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K314" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Five9</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Vice President, Engineering and AI Innovations</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K315" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Flex</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Fw: New jobs similar to Head Of Engineering</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K316" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Fractal</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Head of Engineering - Healthcare &amp; Life Sciences</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K317" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>GNC</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Vice President of Application Engineering</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K318" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>HCA Healthcare</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Chief Information Officer Galen College of Nursing</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K319" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>IDEAYA Biosciences</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Senior Vice President, Information Technology</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K320" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Memorial Sloan Kettering Cancer Center</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Chief Medical Information Officer (CMIO)</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K321" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Mission Critical Materials</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Chief Technical Officer</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K322" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>RealTime eClinical Solutions</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>VP of Software Engineering</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K323" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Sully.ai</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Head of Engineering</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K324" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>The Pittsburgh Foundation</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Chief Information Officer</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K325" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>UpcycleX</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Head of Engineering</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K326" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Banyan Software</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Head of Technology</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K327" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>DrFirst,</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Vice President, Application Development</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K328" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Lensa</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Chief Technology Officer</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K329" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Lensa</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>SVP, CIO (Chief Information Officer)</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K330" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Henry Schein One</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>SVP, Software Engineering</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K331" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr"/>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Abacus Insights</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>AI Engineering Leader</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>Stretch</t>
+        </is>
+      </c>
+      <c r="K332" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr"/>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Jobgether</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Remote Engineering Manager Position</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K333" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr"/>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>iVoyant</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Software Engineering Manager</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K334" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr"/>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Jobgether</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Fw: New jobs similar to Head Of Software Engineering - REMOTE</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K335" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr"/>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Castlight Health</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Associate Director Engineering</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K336" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr"/>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>A Place for Mom</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>Senior Director, Engineering - Senior Living</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K337" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr"/>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>AutoPylot</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>Head of Engineering</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K338" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr"/>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Forward Financing</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Engineering Manager</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K339" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr"/>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Mira Energy Group,</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Chief Technology Officer</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K340" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr"/>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Motional</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Senior Director, Engineering</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K341" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr"/>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>NinjaOne</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>Manager, Software Engineering</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K342" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr"/>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Paradigm Health</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Director, Software Engineering</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K343" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr"/>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Perfecting Peds</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>Director of Engineering</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K344" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr"/>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>REVEL SEARCH®</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Director of Software Engineering</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K345" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr"/>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Ventra Health</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Head of AI and Automation</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K346" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr"/>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Vice President of</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>Sroa Capital and others are hiring for Vice President of Technology in and around West Palm Beach, FL</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K347" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr"/>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>X4 Life Sciences</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>Chief Product &amp; Technology Officer</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>Email Pipeline</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>Pending Review</t>
+        </is>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>Long Shot</t>
+        </is>
+      </c>
+      <c r="K348" t="inlineStr">
+        <is>
+          <t>Sourced via email pipeline</t>
         </is>
       </c>
     </row>

</xml_diff>